<commit_message>
Added PROVIDE ontology processing files
</commit_message>
<xml_diff>
--- a/Load/ontology/Gates/PROVIDE/doc/PROVIDE_aggregated_detection_template.xlsx
+++ b/Load/ontology/Gates/PROVIDE/doc/PROVIDE_aggregated_detection_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/Gates/PROVIDE/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD61DDB-AD90-2445-B2AC-B535E7668D7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC2572-21C8-884F-AC43-BE3D50D630C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22560" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="2100" windowWidth="22560" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
@@ -109,19 +109,19 @@
     <t>Poliovirus serotype 1</t>
   </si>
   <si>
-    <t>ext_mgmt_psi1::s1_mean_burden</t>
-  </si>
-  <si>
-    <t>ext_mgmt_psi2::s2_mean_burden</t>
-  </si>
-  <si>
-    <t>ext_mgmt_psi3::s3_mean_burden</t>
-  </si>
-  <si>
     <t>Poliovirus serotype 2</t>
   </si>
   <si>
     <t>Poliovirus serotype 3</t>
+  </si>
+  <si>
+    <t>ext_mgmt_psi1_2_3::s1_mean_burden</t>
+  </si>
+  <si>
+    <t>ext_mgmt_psi1_2_3::s2_mean_burden</t>
+  </si>
+  <si>
+    <t>ext_mgmt_psi1_2_3::s3_mean_burden</t>
   </si>
 </sst>
 </file>
@@ -973,10 +973,10 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="52" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="3" spans="1:19" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="4" spans="1:19" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
@@ -1139,7 +1139,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N4" s="2" t="str">
         <f t="shared" ref="N4:N10" si="0">TRIM(IF($D4&lt;&gt;"","Mean ","Any ")&amp;IF($H4="",$G4,"")
@@ -1166,7 +1166,7 @@
     </row>
     <row r="5" spans="1:19" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -1184,7 +1184,7 @@
         <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N5" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>